<commit_message>
update to ontwikkel and oefen schema
</commit_message>
<xml_diff>
--- a/templates/oefen/oefen_opdracht_template.xlsx
+++ b/templates/oefen/oefen_opdracht_template.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6315" uniqueCount="1722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6387" uniqueCount="1750">
   <si>
     <t>naam</t>
   </si>
@@ -4466,6 +4466,30 @@
     <t>R471811</t>
   </si>
   <si>
+    <t>VESS</t>
+  </si>
+  <si>
+    <t>VeldCap</t>
+  </si>
+  <si>
+    <t>TBV</t>
+  </si>
+  <si>
+    <t>pos_akker</t>
+  </si>
+  <si>
+    <t>pF-curve</t>
+  </si>
+  <si>
+    <t>pF4.25</t>
+  </si>
+  <si>
+    <t>pF</t>
+  </si>
+  <si>
+    <t>DW</t>
+  </si>
+  <si>
     <t>voorbehandeling_observatie_type_bewaring</t>
   </si>
   <si>
@@ -5138,6 +5162,66 @@
     <t>CMA_2_I_A.2 - Electrische geleidbaarheid</t>
   </si>
   <si>
+    <t>zandbakapparaat en drukkamers</t>
+  </si>
+  <si>
+    <t>Double Spade VESS (DSVESS), 7 criteria</t>
+  </si>
+  <si>
+    <t>Double Spade VESS (DSVESS), 3 criteria</t>
+  </si>
+  <si>
+    <t>HYPROP® aangepaste verdampingsmethode (METER Group, Schindler et al., 2010)</t>
+  </si>
+  <si>
+    <t>SST (pF0-2); KST (pF2.3-2.7); PMC (pF3.4 -4.2); PPE (pF3.4 -4.2)</t>
+  </si>
+  <si>
+    <t>Zeefrest 2 mm</t>
+  </si>
+  <si>
+    <t>Laserdiffractometer (Coulter LS2000, ISO 11277)</t>
+  </si>
+  <si>
+    <t>Textuur pipetmethode Robinson-Köhn volgens CMA/2/II/A.6 (toegepast voor alle fracties)</t>
+  </si>
+  <si>
+    <t>Waterretentiecurve - gemeten</t>
+  </si>
+  <si>
+    <t>Parametrische PTF - gemodelleerd</t>
+  </si>
+  <si>
+    <t>Parametrische PTF - gemodelleerd (studie vochtretentiecapaciteit)</t>
+  </si>
+  <si>
+    <t>afgeleid met behulp van de Belgische textuurdriehoek uit fracties zand/leem/klei gemeten met behulp van de pipet/zeefmethode</t>
+  </si>
+  <si>
+    <t>afgeleid met behulp van de Belgische textuurdriehoek uit fracties zand/leem/klei gemeten met behulp van de laserdiffractie</t>
+  </si>
+  <si>
+    <t>pipet/zeefmethode (Gee &amp; Bauder, 1986) (ISO 11277)</t>
+  </si>
+  <si>
+    <t>pH in KCl, 1:5 (V/V) (ISO10390)</t>
+  </si>
+  <si>
+    <t>pH in KCl, 1:2 (V/V) (ISO10390)</t>
+  </si>
+  <si>
+    <t>Visuele beoordeling</t>
+  </si>
+  <si>
+    <t>Proefplan testveld</t>
+  </si>
+  <si>
+    <t>ringmethode (Dirksen, 1999)</t>
+  </si>
+  <si>
+    <t>ringmethode (Grossman &amp; Reinsch, 2002)</t>
+  </si>
+  <si>
     <t>https://data.bodemenondergrond.vlaanderen.be/id/concept/betrouwbaarheid/A</t>
   </si>
   <si>
@@ -5153,13 +5237,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-08-06 15:10:55.559620</t>
+    <t>2025-09-18 15:21:12.079267</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.1.6</t>
+    <t>2.1.7</t>
   </si>
   <si>
     <t>xdov-version</t>
@@ -5328,7 +5412,7 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="W3:X995" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="W3:X1003" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -5378,7 +5462,7 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="AG3:AH161" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="AG3:AH181" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -5398,7 +5482,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="AK3:AL995" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="AK3:AL1003" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -5792,7 +5876,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP995"/>
+  <dimension ref="A1:AP1003"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5829,7 +5913,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1" t="s">
-        <v>1709</v>
+        <v>1737</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -6139,37 +6223,37 @@
         <v>42</v>
       </c>
       <c r="Y4" t="s">
-        <v>1487</v>
+        <v>1495</v>
       </c>
       <c r="Z4" t="s">
         <v>42</v>
       </c>
       <c r="AA4" t="s">
-        <v>1487</v>
+        <v>1495</v>
       </c>
       <c r="AB4" t="s">
         <v>42</v>
       </c>
       <c r="AC4" t="s">
-        <v>1487</v>
+        <v>1495</v>
       </c>
       <c r="AD4" t="s">
         <v>42</v>
       </c>
       <c r="AE4" t="s">
-        <v>1550</v>
+        <v>1558</v>
       </c>
       <c r="AF4" t="s">
         <v>42</v>
       </c>
       <c r="AG4" t="s">
-        <v>1552</v>
+        <v>1560</v>
       </c>
       <c r="AH4" t="s">
         <v>42</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>1706</v>
+        <v>1734</v>
       </c>
       <c r="AJ4" t="s">
         <v>42</v>
@@ -6181,7 +6265,7 @@
         <v>42</v>
       </c>
       <c r="AM4" t="s">
-        <v>1487</v>
+        <v>1495</v>
       </c>
       <c r="AN4" t="s">
         <v>42</v>
@@ -6267,37 +6351,37 @@
         <v>42</v>
       </c>
       <c r="Y5" t="s">
-        <v>1488</v>
+        <v>1496</v>
       </c>
       <c r="Z5" t="s">
         <v>42</v>
       </c>
       <c r="AA5" t="s">
-        <v>1488</v>
+        <v>1496</v>
       </c>
       <c r="AB5" t="s">
         <v>42</v>
       </c>
       <c r="AC5" t="s">
-        <v>1488</v>
+        <v>1496</v>
       </c>
       <c r="AD5" t="s">
         <v>42</v>
       </c>
       <c r="AE5" t="s">
-        <v>1551</v>
+        <v>1559</v>
       </c>
       <c r="AF5" t="s">
         <v>42</v>
       </c>
       <c r="AG5" t="s">
-        <v>1553</v>
+        <v>1561</v>
       </c>
       <c r="AH5" t="s">
         <v>42</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>1707</v>
+        <v>1735</v>
       </c>
       <c r="AJ5" t="s">
         <v>42</v>
@@ -6309,7 +6393,7 @@
         <v>42</v>
       </c>
       <c r="AM5" t="s">
-        <v>1488</v>
+        <v>1496</v>
       </c>
       <c r="AN5" t="s">
         <v>42</v>
@@ -6389,37 +6473,37 @@
         <v>42</v>
       </c>
       <c r="Y6" t="s">
-        <v>1489</v>
+        <v>1497</v>
       </c>
       <c r="Z6" t="s">
         <v>42</v>
       </c>
       <c r="AA6" t="s">
-        <v>1489</v>
+        <v>1497</v>
       </c>
       <c r="AB6" t="s">
         <v>42</v>
       </c>
       <c r="AC6" t="s">
-        <v>1489</v>
+        <v>1497</v>
       </c>
       <c r="AD6" t="s">
         <v>42</v>
       </c>
       <c r="AE6" t="s">
-        <v>1487</v>
+        <v>1495</v>
       </c>
       <c r="AF6" t="s">
         <v>42</v>
       </c>
       <c r="AG6" t="s">
-        <v>1554</v>
+        <v>1562</v>
       </c>
       <c r="AH6" t="s">
         <v>42</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>1708</v>
+        <v>1736</v>
       </c>
       <c r="AJ6" t="s">
         <v>42</v>
@@ -6431,7 +6515,7 @@
         <v>42</v>
       </c>
       <c r="AM6" t="s">
-        <v>1489</v>
+        <v>1497</v>
       </c>
       <c r="AN6" t="s">
         <v>42</v>
@@ -6505,25 +6589,25 @@
         <v>42</v>
       </c>
       <c r="Y7" t="s">
-        <v>1490</v>
+        <v>1498</v>
       </c>
       <c r="Z7" t="s">
         <v>42</v>
       </c>
       <c r="AA7" t="s">
-        <v>1490</v>
+        <v>1498</v>
       </c>
       <c r="AB7" t="s">
         <v>42</v>
       </c>
       <c r="AC7" t="s">
-        <v>1490</v>
+        <v>1498</v>
       </c>
       <c r="AD7" t="s">
         <v>42</v>
       </c>
       <c r="AG7" t="s">
-        <v>1555</v>
+        <v>1563</v>
       </c>
       <c r="AH7" t="s">
         <v>42</v>
@@ -6535,7 +6619,7 @@
         <v>42</v>
       </c>
       <c r="AM7" t="s">
-        <v>1490</v>
+        <v>1498</v>
       </c>
       <c r="AN7" t="s">
         <v>42</v>
@@ -6609,25 +6693,25 @@
         <v>42</v>
       </c>
       <c r="Y8" t="s">
-        <v>1491</v>
+        <v>1499</v>
       </c>
       <c r="Z8" t="s">
         <v>42</v>
       </c>
       <c r="AA8" t="s">
-        <v>1491</v>
+        <v>1499</v>
       </c>
       <c r="AB8" t="s">
         <v>42</v>
       </c>
       <c r="AC8" t="s">
-        <v>1491</v>
+        <v>1499</v>
       </c>
       <c r="AD8" t="s">
         <v>42</v>
       </c>
       <c r="AG8" t="s">
-        <v>1556</v>
+        <v>1564</v>
       </c>
       <c r="AH8" t="s">
         <v>42</v>
@@ -6639,7 +6723,7 @@
         <v>42</v>
       </c>
       <c r="AM8" t="s">
-        <v>1491</v>
+        <v>1499</v>
       </c>
       <c r="AN8" t="s">
         <v>42</v>
@@ -6707,25 +6791,25 @@
         <v>42</v>
       </c>
       <c r="Y9" t="s">
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="Z9" t="s">
         <v>42</v>
       </c>
       <c r="AA9" t="s">
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="AB9" t="s">
         <v>42</v>
       </c>
       <c r="AC9" t="s">
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="AD9" t="s">
         <v>42</v>
       </c>
       <c r="AG9" t="s">
-        <v>1557</v>
+        <v>1565</v>
       </c>
       <c r="AH9" t="s">
         <v>42</v>
@@ -6737,7 +6821,7 @@
         <v>42</v>
       </c>
       <c r="AM9" t="s">
-        <v>1492</v>
+        <v>1500</v>
       </c>
       <c r="AN9" t="s">
         <v>42</v>
@@ -6805,25 +6889,25 @@
         <v>42</v>
       </c>
       <c r="Y10" t="s">
-        <v>1493</v>
+        <v>1501</v>
       </c>
       <c r="Z10" t="s">
         <v>42</v>
       </c>
       <c r="AA10" t="s">
-        <v>1493</v>
+        <v>1501</v>
       </c>
       <c r="AB10" t="s">
         <v>42</v>
       </c>
       <c r="AC10" t="s">
-        <v>1493</v>
+        <v>1501</v>
       </c>
       <c r="AD10" t="s">
         <v>42</v>
       </c>
       <c r="AG10" t="s">
-        <v>1558</v>
+        <v>1566</v>
       </c>
       <c r="AH10" t="s">
         <v>42</v>
@@ -6835,7 +6919,7 @@
         <v>42</v>
       </c>
       <c r="AM10" t="s">
-        <v>1493</v>
+        <v>1501</v>
       </c>
       <c r="AN10" t="s">
         <v>42</v>
@@ -6903,25 +6987,25 @@
         <v>42</v>
       </c>
       <c r="Y11" t="s">
-        <v>1494</v>
+        <v>1502</v>
       </c>
       <c r="Z11" t="s">
         <v>42</v>
       </c>
       <c r="AA11" t="s">
-        <v>1494</v>
+        <v>1502</v>
       </c>
       <c r="AB11" t="s">
         <v>42</v>
       </c>
       <c r="AC11" t="s">
-        <v>1494</v>
+        <v>1502</v>
       </c>
       <c r="AD11" t="s">
         <v>42</v>
       </c>
       <c r="AG11" t="s">
-        <v>1559</v>
+        <v>1567</v>
       </c>
       <c r="AH11" t="s">
         <v>42</v>
@@ -6933,7 +7017,7 @@
         <v>42</v>
       </c>
       <c r="AM11" t="s">
-        <v>1494</v>
+        <v>1502</v>
       </c>
       <c r="AN11" t="s">
         <v>42</v>
@@ -7001,25 +7085,25 @@
         <v>42</v>
       </c>
       <c r="Y12" t="s">
-        <v>1495</v>
+        <v>1503</v>
       </c>
       <c r="Z12" t="s">
         <v>42</v>
       </c>
       <c r="AA12" t="s">
-        <v>1495</v>
+        <v>1503</v>
       </c>
       <c r="AB12" t="s">
         <v>42</v>
       </c>
       <c r="AC12" t="s">
-        <v>1495</v>
+        <v>1503</v>
       </c>
       <c r="AD12" t="s">
         <v>42</v>
       </c>
       <c r="AG12" t="s">
-        <v>1560</v>
+        <v>1568</v>
       </c>
       <c r="AH12" t="s">
         <v>42</v>
@@ -7031,7 +7115,7 @@
         <v>42</v>
       </c>
       <c r="AM12" t="s">
-        <v>1495</v>
+        <v>1503</v>
       </c>
       <c r="AN12" t="s">
         <v>42</v>
@@ -7093,25 +7177,25 @@
         <v>42</v>
       </c>
       <c r="Y13" t="s">
-        <v>1496</v>
+        <v>1504</v>
       </c>
       <c r="Z13" t="s">
         <v>42</v>
       </c>
       <c r="AA13" t="s">
-        <v>1496</v>
+        <v>1504</v>
       </c>
       <c r="AB13" t="s">
         <v>42</v>
       </c>
       <c r="AC13" t="s">
-        <v>1496</v>
+        <v>1504</v>
       </c>
       <c r="AD13" t="s">
         <v>42</v>
       </c>
       <c r="AG13" t="s">
-        <v>1561</v>
+        <v>1569</v>
       </c>
       <c r="AH13" t="s">
         <v>42</v>
@@ -7123,7 +7207,7 @@
         <v>42</v>
       </c>
       <c r="AM13" t="s">
-        <v>1496</v>
+        <v>1504</v>
       </c>
       <c r="AN13" t="s">
         <v>42</v>
@@ -7185,25 +7269,25 @@
         <v>42</v>
       </c>
       <c r="Y14" t="s">
-        <v>1497</v>
+        <v>1505</v>
       </c>
       <c r="Z14" t="s">
         <v>42</v>
       </c>
       <c r="AA14" t="s">
-        <v>1497</v>
+        <v>1505</v>
       </c>
       <c r="AB14" t="s">
         <v>42</v>
       </c>
       <c r="AC14" t="s">
-        <v>1497</v>
+        <v>1505</v>
       </c>
       <c r="AD14" t="s">
         <v>42</v>
       </c>
       <c r="AG14" t="s">
-        <v>1562</v>
+        <v>1570</v>
       </c>
       <c r="AH14" t="s">
         <v>42</v>
@@ -7215,7 +7299,7 @@
         <v>42</v>
       </c>
       <c r="AM14" t="s">
-        <v>1497</v>
+        <v>1505</v>
       </c>
       <c r="AN14" t="s">
         <v>42</v>
@@ -7271,25 +7355,25 @@
         <v>42</v>
       </c>
       <c r="Y15" t="s">
-        <v>1498</v>
+        <v>1506</v>
       </c>
       <c r="Z15" t="s">
         <v>42</v>
       </c>
       <c r="AA15" t="s">
-        <v>1498</v>
+        <v>1506</v>
       </c>
       <c r="AB15" t="s">
         <v>42</v>
       </c>
       <c r="AC15" t="s">
-        <v>1498</v>
+        <v>1506</v>
       </c>
       <c r="AD15" t="s">
         <v>42</v>
       </c>
       <c r="AG15" t="s">
-        <v>1563</v>
+        <v>1571</v>
       </c>
       <c r="AH15" t="s">
         <v>42</v>
@@ -7301,7 +7385,7 @@
         <v>42</v>
       </c>
       <c r="AM15" t="s">
-        <v>1498</v>
+        <v>1506</v>
       </c>
       <c r="AN15" t="s">
         <v>42</v>
@@ -7357,25 +7441,25 @@
         <v>42</v>
       </c>
       <c r="Y16" t="s">
-        <v>1499</v>
+        <v>1507</v>
       </c>
       <c r="Z16" t="s">
         <v>42</v>
       </c>
       <c r="AA16" t="s">
-        <v>1499</v>
+        <v>1507</v>
       </c>
       <c r="AB16" t="s">
         <v>42</v>
       </c>
       <c r="AC16" t="s">
-        <v>1499</v>
+        <v>1507</v>
       </c>
       <c r="AD16" t="s">
         <v>42</v>
       </c>
       <c r="AG16" t="s">
-        <v>1564</v>
+        <v>1572</v>
       </c>
       <c r="AH16" t="s">
         <v>42</v>
@@ -7387,7 +7471,7 @@
         <v>42</v>
       </c>
       <c r="AM16" t="s">
-        <v>1499</v>
+        <v>1507</v>
       </c>
       <c r="AN16" t="s">
         <v>42</v>
@@ -7443,25 +7527,25 @@
         <v>42</v>
       </c>
       <c r="Y17" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
       <c r="Z17" t="s">
         <v>42</v>
       </c>
       <c r="AA17" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
       <c r="AB17" t="s">
         <v>42</v>
       </c>
       <c r="AC17" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
       <c r="AD17" t="s">
         <v>42</v>
       </c>
       <c r="AG17" t="s">
-        <v>1565</v>
+        <v>1573</v>
       </c>
       <c r="AH17" t="s">
         <v>42</v>
@@ -7473,7 +7557,7 @@
         <v>42</v>
       </c>
       <c r="AM17" t="s">
-        <v>1500</v>
+        <v>1508</v>
       </c>
       <c r="AN17" t="s">
         <v>42</v>
@@ -7529,25 +7613,25 @@
         <v>42</v>
       </c>
       <c r="Y18" t="s">
-        <v>1501</v>
+        <v>1509</v>
       </c>
       <c r="Z18" t="s">
         <v>42</v>
       </c>
       <c r="AA18" t="s">
-        <v>1501</v>
+        <v>1509</v>
       </c>
       <c r="AB18" t="s">
         <v>42</v>
       </c>
       <c r="AC18" t="s">
-        <v>1501</v>
+        <v>1509</v>
       </c>
       <c r="AD18" t="s">
         <v>42</v>
       </c>
       <c r="AG18" t="s">
-        <v>1566</v>
+        <v>1574</v>
       </c>
       <c r="AH18" t="s">
         <v>42</v>
@@ -7559,7 +7643,7 @@
         <v>42</v>
       </c>
       <c r="AM18" t="s">
-        <v>1501</v>
+        <v>1509</v>
       </c>
       <c r="AN18" t="s">
         <v>42</v>
@@ -7609,19 +7693,19 @@
         <v>42</v>
       </c>
       <c r="Y19" t="s">
-        <v>1502</v>
+        <v>1510</v>
       </c>
       <c r="Z19" t="s">
         <v>42</v>
       </c>
       <c r="AA19" t="s">
-        <v>1502</v>
+        <v>1510</v>
       </c>
       <c r="AB19" t="s">
         <v>42</v>
       </c>
       <c r="AC19" t="s">
-        <v>1502</v>
+        <v>1510</v>
       </c>
       <c r="AD19" t="s">
         <v>42</v>
@@ -7639,7 +7723,7 @@
         <v>42</v>
       </c>
       <c r="AM19" t="s">
-        <v>1502</v>
+        <v>1510</v>
       </c>
       <c r="AN19" t="s">
         <v>42</v>
@@ -7689,25 +7773,25 @@
         <v>42</v>
       </c>
       <c r="Y20" t="s">
-        <v>1503</v>
+        <v>1511</v>
       </c>
       <c r="Z20" t="s">
         <v>42</v>
       </c>
       <c r="AA20" t="s">
-        <v>1503</v>
+        <v>1511</v>
       </c>
       <c r="AB20" t="s">
         <v>42</v>
       </c>
       <c r="AC20" t="s">
-        <v>1503</v>
+        <v>1511</v>
       </c>
       <c r="AD20" t="s">
         <v>42</v>
       </c>
       <c r="AG20" t="s">
-        <v>1567</v>
+        <v>1575</v>
       </c>
       <c r="AH20" t="s">
         <v>42</v>
@@ -7719,7 +7803,7 @@
         <v>42</v>
       </c>
       <c r="AM20" t="s">
-        <v>1503</v>
+        <v>1511</v>
       </c>
       <c r="AN20" t="s">
         <v>42</v>
@@ -7769,25 +7853,25 @@
         <v>42</v>
       </c>
       <c r="Y21" t="s">
-        <v>1504</v>
+        <v>1512</v>
       </c>
       <c r="Z21" t="s">
         <v>42</v>
       </c>
       <c r="AA21" t="s">
-        <v>1504</v>
+        <v>1512</v>
       </c>
       <c r="AB21" t="s">
         <v>42</v>
       </c>
       <c r="AC21" t="s">
-        <v>1504</v>
+        <v>1512</v>
       </c>
       <c r="AD21" t="s">
         <v>42</v>
       </c>
       <c r="AG21" t="s">
-        <v>1568</v>
+        <v>1576</v>
       </c>
       <c r="AH21" t="s">
         <v>42</v>
@@ -7799,7 +7883,7 @@
         <v>42</v>
       </c>
       <c r="AM21" t="s">
-        <v>1504</v>
+        <v>1512</v>
       </c>
       <c r="AN21" t="s">
         <v>42</v>
@@ -7849,25 +7933,25 @@
         <v>42</v>
       </c>
       <c r="Y22" t="s">
-        <v>1505</v>
+        <v>1513</v>
       </c>
       <c r="Z22" t="s">
         <v>42</v>
       </c>
       <c r="AA22" t="s">
-        <v>1505</v>
+        <v>1513</v>
       </c>
       <c r="AB22" t="s">
         <v>42</v>
       </c>
       <c r="AC22" t="s">
-        <v>1505</v>
+        <v>1513</v>
       </c>
       <c r="AD22" t="s">
         <v>42</v>
       </c>
       <c r="AG22" t="s">
-        <v>1569</v>
+        <v>1577</v>
       </c>
       <c r="AH22" t="s">
         <v>42</v>
@@ -7879,7 +7963,7 @@
         <v>42</v>
       </c>
       <c r="AM22" t="s">
-        <v>1505</v>
+        <v>1513</v>
       </c>
       <c r="AN22" t="s">
         <v>42</v>
@@ -7929,25 +8013,25 @@
         <v>42</v>
       </c>
       <c r="Y23" t="s">
-        <v>1506</v>
+        <v>1514</v>
       </c>
       <c r="Z23" t="s">
         <v>42</v>
       </c>
       <c r="AA23" t="s">
-        <v>1506</v>
+        <v>1514</v>
       </c>
       <c r="AB23" t="s">
         <v>42</v>
       </c>
       <c r="AC23" t="s">
-        <v>1506</v>
+        <v>1514</v>
       </c>
       <c r="AD23" t="s">
         <v>42</v>
       </c>
       <c r="AG23" t="s">
-        <v>1570</v>
+        <v>1578</v>
       </c>
       <c r="AH23" t="s">
         <v>42</v>
@@ -7959,7 +8043,7 @@
         <v>42</v>
       </c>
       <c r="AM23" t="s">
-        <v>1506</v>
+        <v>1514</v>
       </c>
       <c r="AN23" t="s">
         <v>42</v>
@@ -8027,7 +8111,7 @@
         <v>42</v>
       </c>
       <c r="AG24" t="s">
-        <v>1571</v>
+        <v>1579</v>
       </c>
       <c r="AH24" t="s">
         <v>42</v>
@@ -8089,25 +8173,25 @@
         <v>42</v>
       </c>
       <c r="Y25" t="s">
-        <v>1507</v>
+        <v>1515</v>
       </c>
       <c r="Z25" t="s">
         <v>42</v>
       </c>
       <c r="AA25" t="s">
-        <v>1507</v>
+        <v>1515</v>
       </c>
       <c r="AB25" t="s">
         <v>42</v>
       </c>
       <c r="AC25" t="s">
-        <v>1507</v>
+        <v>1515</v>
       </c>
       <c r="AD25" t="s">
         <v>42</v>
       </c>
       <c r="AG25" t="s">
-        <v>1572</v>
+        <v>1580</v>
       </c>
       <c r="AH25" t="s">
         <v>42</v>
@@ -8119,7 +8203,7 @@
         <v>42</v>
       </c>
       <c r="AM25" t="s">
-        <v>1507</v>
+        <v>1515</v>
       </c>
       <c r="AN25" t="s">
         <v>42</v>
@@ -8169,25 +8253,25 @@
         <v>42</v>
       </c>
       <c r="Y26" t="s">
-        <v>1508</v>
+        <v>1516</v>
       </c>
       <c r="Z26" t="s">
         <v>42</v>
       </c>
       <c r="AA26" t="s">
-        <v>1508</v>
+        <v>1516</v>
       </c>
       <c r="AB26" t="s">
         <v>42</v>
       </c>
       <c r="AC26" t="s">
-        <v>1508</v>
+        <v>1516</v>
       </c>
       <c r="AD26" t="s">
         <v>42</v>
       </c>
       <c r="AG26" t="s">
-        <v>1573</v>
+        <v>1581</v>
       </c>
       <c r="AH26" t="s">
         <v>42</v>
@@ -8199,7 +8283,7 @@
         <v>42</v>
       </c>
       <c r="AM26" t="s">
-        <v>1508</v>
+        <v>1516</v>
       </c>
       <c r="AN26" t="s">
         <v>42</v>
@@ -8249,25 +8333,25 @@
         <v>42</v>
       </c>
       <c r="Y27" t="s">
-        <v>1509</v>
+        <v>1517</v>
       </c>
       <c r="Z27" t="s">
         <v>42</v>
       </c>
       <c r="AA27" t="s">
-        <v>1509</v>
+        <v>1517</v>
       </c>
       <c r="AB27" t="s">
         <v>42</v>
       </c>
       <c r="AC27" t="s">
-        <v>1509</v>
+        <v>1517</v>
       </c>
       <c r="AD27" t="s">
         <v>42</v>
       </c>
       <c r="AG27" t="s">
-        <v>1574</v>
+        <v>1582</v>
       </c>
       <c r="AH27" t="s">
         <v>42</v>
@@ -8279,7 +8363,7 @@
         <v>42</v>
       </c>
       <c r="AM27" t="s">
-        <v>1509</v>
+        <v>1517</v>
       </c>
       <c r="AN27" t="s">
         <v>42</v>
@@ -8329,25 +8413,25 @@
         <v>42</v>
       </c>
       <c r="Y28" t="s">
-        <v>1510</v>
+        <v>1518</v>
       </c>
       <c r="Z28" t="s">
         <v>42</v>
       </c>
       <c r="AA28" t="s">
-        <v>1510</v>
+        <v>1518</v>
       </c>
       <c r="AB28" t="s">
         <v>42</v>
       </c>
       <c r="AC28" t="s">
-        <v>1510</v>
+        <v>1518</v>
       </c>
       <c r="AD28" t="s">
         <v>42</v>
       </c>
       <c r="AG28" t="s">
-        <v>1575</v>
+        <v>1583</v>
       </c>
       <c r="AH28" t="s">
         <v>42</v>
@@ -8359,7 +8443,7 @@
         <v>42</v>
       </c>
       <c r="AM28" t="s">
-        <v>1510</v>
+        <v>1518</v>
       </c>
       <c r="AN28" t="s">
         <v>42</v>
@@ -8409,25 +8493,25 @@
         <v>42</v>
       </c>
       <c r="Y29" t="s">
-        <v>1511</v>
+        <v>1519</v>
       </c>
       <c r="Z29" t="s">
         <v>42</v>
       </c>
       <c r="AA29" t="s">
-        <v>1511</v>
+        <v>1519</v>
       </c>
       <c r="AB29" t="s">
         <v>42</v>
       </c>
       <c r="AC29" t="s">
-        <v>1511</v>
+        <v>1519</v>
       </c>
       <c r="AD29" t="s">
         <v>42</v>
       </c>
       <c r="AG29" t="s">
-        <v>1576</v>
+        <v>1584</v>
       </c>
       <c r="AH29" t="s">
         <v>42</v>
@@ -8439,7 +8523,7 @@
         <v>42</v>
       </c>
       <c r="AM29" t="s">
-        <v>1511</v>
+        <v>1519</v>
       </c>
       <c r="AN29" t="s">
         <v>42</v>
@@ -8483,25 +8567,25 @@
         <v>42</v>
       </c>
       <c r="Y30" t="s">
-        <v>1512</v>
+        <v>1520</v>
       </c>
       <c r="Z30" t="s">
         <v>42</v>
       </c>
       <c r="AA30" t="s">
-        <v>1512</v>
+        <v>1520</v>
       </c>
       <c r="AB30" t="s">
         <v>42</v>
       </c>
       <c r="AC30" t="s">
-        <v>1512</v>
+        <v>1520</v>
       </c>
       <c r="AD30" t="s">
         <v>42</v>
       </c>
       <c r="AG30" t="s">
-        <v>1577</v>
+        <v>1585</v>
       </c>
       <c r="AH30" t="s">
         <v>42</v>
@@ -8513,7 +8597,7 @@
         <v>42</v>
       </c>
       <c r="AM30" t="s">
-        <v>1512</v>
+        <v>1520</v>
       </c>
       <c r="AN30" t="s">
         <v>42</v>
@@ -8557,25 +8641,25 @@
         <v>42</v>
       </c>
       <c r="Y31" t="s">
-        <v>1513</v>
+        <v>1521</v>
       </c>
       <c r="Z31" t="s">
         <v>42</v>
       </c>
       <c r="AA31" t="s">
-        <v>1513</v>
+        <v>1521</v>
       </c>
       <c r="AB31" t="s">
         <v>42</v>
       </c>
       <c r="AC31" t="s">
-        <v>1513</v>
+        <v>1521</v>
       </c>
       <c r="AD31" t="s">
         <v>42</v>
       </c>
       <c r="AG31" t="s">
-        <v>1578</v>
+        <v>1586</v>
       </c>
       <c r="AH31" t="s">
         <v>42</v>
@@ -8587,7 +8671,7 @@
         <v>42</v>
       </c>
       <c r="AM31" t="s">
-        <v>1513</v>
+        <v>1521</v>
       </c>
       <c r="AN31" t="s">
         <v>42</v>
@@ -8631,25 +8715,25 @@
         <v>42</v>
       </c>
       <c r="Y32" t="s">
-        <v>1514</v>
+        <v>1522</v>
       </c>
       <c r="Z32" t="s">
         <v>42</v>
       </c>
       <c r="AA32" t="s">
-        <v>1514</v>
+        <v>1522</v>
       </c>
       <c r="AB32" t="s">
         <v>42</v>
       </c>
       <c r="AC32" t="s">
-        <v>1514</v>
+        <v>1522</v>
       </c>
       <c r="AD32" t="s">
         <v>42</v>
       </c>
       <c r="AG32" t="s">
-        <v>1579</v>
+        <v>1587</v>
       </c>
       <c r="AH32" t="s">
         <v>42</v>
@@ -8661,7 +8745,7 @@
         <v>42</v>
       </c>
       <c r="AM32" t="s">
-        <v>1514</v>
+        <v>1522</v>
       </c>
       <c r="AN32" t="s">
         <v>42</v>
@@ -8705,25 +8789,25 @@
         <v>42</v>
       </c>
       <c r="Y33" t="s">
-        <v>1515</v>
+        <v>1523</v>
       </c>
       <c r="Z33" t="s">
         <v>42</v>
       </c>
       <c r="AA33" t="s">
-        <v>1515</v>
+        <v>1523</v>
       </c>
       <c r="AB33" t="s">
         <v>42</v>
       </c>
       <c r="AC33" t="s">
-        <v>1515</v>
+        <v>1523</v>
       </c>
       <c r="AD33" t="s">
         <v>42</v>
       </c>
       <c r="AG33" t="s">
-        <v>1580</v>
+        <v>1588</v>
       </c>
       <c r="AH33" t="s">
         <v>42</v>
@@ -8735,7 +8819,7 @@
         <v>42</v>
       </c>
       <c r="AM33" t="s">
-        <v>1515</v>
+        <v>1523</v>
       </c>
       <c r="AN33" t="s">
         <v>42</v>
@@ -8779,25 +8863,25 @@
         <v>42</v>
       </c>
       <c r="Y34" t="s">
-        <v>1516</v>
+        <v>1524</v>
       </c>
       <c r="Z34" t="s">
         <v>42</v>
       </c>
       <c r="AA34" t="s">
-        <v>1516</v>
+        <v>1524</v>
       </c>
       <c r="AB34" t="s">
         <v>42</v>
       </c>
       <c r="AC34" t="s">
-        <v>1516</v>
+        <v>1524</v>
       </c>
       <c r="AD34" t="s">
         <v>42</v>
       </c>
       <c r="AG34" t="s">
-        <v>1581</v>
+        <v>1589</v>
       </c>
       <c r="AH34" t="s">
         <v>42</v>
@@ -8809,7 +8893,7 @@
         <v>42</v>
       </c>
       <c r="AM34" t="s">
-        <v>1516</v>
+        <v>1524</v>
       </c>
       <c r="AN34" t="s">
         <v>42</v>
@@ -8853,25 +8937,25 @@
         <v>42</v>
       </c>
       <c r="Y35" t="s">
-        <v>1517</v>
+        <v>1525</v>
       </c>
       <c r="Z35" t="s">
         <v>42</v>
       </c>
       <c r="AA35" t="s">
-        <v>1517</v>
+        <v>1525</v>
       </c>
       <c r="AB35" t="s">
         <v>42</v>
       </c>
       <c r="AC35" t="s">
-        <v>1517</v>
+        <v>1525</v>
       </c>
       <c r="AD35" t="s">
         <v>42</v>
       </c>
       <c r="AG35" t="s">
-        <v>1582</v>
+        <v>1590</v>
       </c>
       <c r="AH35" t="s">
         <v>42</v>
@@ -8883,7 +8967,7 @@
         <v>42</v>
       </c>
       <c r="AM35" t="s">
-        <v>1517</v>
+        <v>1525</v>
       </c>
       <c r="AN35" t="s">
         <v>42</v>
@@ -8927,25 +9011,25 @@
         <v>42</v>
       </c>
       <c r="Y36" t="s">
-        <v>1518</v>
+        <v>1526</v>
       </c>
       <c r="Z36" t="s">
         <v>42</v>
       </c>
       <c r="AA36" t="s">
-        <v>1518</v>
+        <v>1526</v>
       </c>
       <c r="AB36" t="s">
         <v>42</v>
       </c>
       <c r="AC36" t="s">
-        <v>1518</v>
+        <v>1526</v>
       </c>
       <c r="AD36" t="s">
         <v>42</v>
       </c>
       <c r="AG36" t="s">
-        <v>1583</v>
+        <v>1591</v>
       </c>
       <c r="AH36" t="s">
         <v>42</v>
@@ -8957,7 +9041,7 @@
         <v>42</v>
       </c>
       <c r="AM36" t="s">
-        <v>1518</v>
+        <v>1526</v>
       </c>
       <c r="AN36" t="s">
         <v>42</v>
@@ -9001,25 +9085,25 @@
         <v>42</v>
       </c>
       <c r="Y37" t="s">
-        <v>1519</v>
+        <v>1527</v>
       </c>
       <c r="Z37" t="s">
         <v>42</v>
       </c>
       <c r="AA37" t="s">
-        <v>1519</v>
+        <v>1527</v>
       </c>
       <c r="AB37" t="s">
         <v>42</v>
       </c>
       <c r="AC37" t="s">
-        <v>1519</v>
+        <v>1527</v>
       </c>
       <c r="AD37" t="s">
         <v>42</v>
       </c>
       <c r="AG37" t="s">
-        <v>1584</v>
+        <v>1592</v>
       </c>
       <c r="AH37" t="s">
         <v>42</v>
@@ -9031,7 +9115,7 @@
         <v>42</v>
       </c>
       <c r="AM37" t="s">
-        <v>1519</v>
+        <v>1527</v>
       </c>
       <c r="AN37" t="s">
         <v>42</v>
@@ -9075,25 +9159,25 @@
         <v>42</v>
       </c>
       <c r="Y38" t="s">
-        <v>1520</v>
+        <v>1528</v>
       </c>
       <c r="Z38" t="s">
         <v>42</v>
       </c>
       <c r="AA38" t="s">
-        <v>1520</v>
+        <v>1528</v>
       </c>
       <c r="AB38" t="s">
         <v>42</v>
       </c>
       <c r="AC38" t="s">
-        <v>1520</v>
+        <v>1528</v>
       </c>
       <c r="AD38" t="s">
         <v>42</v>
       </c>
       <c r="AG38" t="s">
-        <v>1585</v>
+        <v>1593</v>
       </c>
       <c r="AH38" t="s">
         <v>42</v>
@@ -9105,7 +9189,7 @@
         <v>42</v>
       </c>
       <c r="AM38" t="s">
-        <v>1520</v>
+        <v>1528</v>
       </c>
       <c r="AN38" t="s">
         <v>42</v>
@@ -9149,25 +9233,25 @@
         <v>42</v>
       </c>
       <c r="Y39" t="s">
-        <v>1521</v>
+        <v>1529</v>
       </c>
       <c r="Z39" t="s">
         <v>42</v>
       </c>
       <c r="AA39" t="s">
-        <v>1521</v>
+        <v>1529</v>
       </c>
       <c r="AB39" t="s">
         <v>42</v>
       </c>
       <c r="AC39" t="s">
-        <v>1521</v>
+        <v>1529</v>
       </c>
       <c r="AD39" t="s">
         <v>42</v>
       </c>
       <c r="AG39" t="s">
-        <v>1586</v>
+        <v>1594</v>
       </c>
       <c r="AH39" t="s">
         <v>42</v>
@@ -9179,7 +9263,7 @@
         <v>42</v>
       </c>
       <c r="AM39" t="s">
-        <v>1521</v>
+        <v>1529</v>
       </c>
       <c r="AN39" t="s">
         <v>42</v>
@@ -9223,25 +9307,25 @@
         <v>42</v>
       </c>
       <c r="Y40" t="s">
-        <v>1522</v>
+        <v>1530</v>
       </c>
       <c r="Z40" t="s">
         <v>42</v>
       </c>
       <c r="AA40" t="s">
-        <v>1522</v>
+        <v>1530</v>
       </c>
       <c r="AB40" t="s">
         <v>42</v>
       </c>
       <c r="AC40" t="s">
-        <v>1522</v>
+        <v>1530</v>
       </c>
       <c r="AD40" t="s">
         <v>42</v>
       </c>
       <c r="AG40" t="s">
-        <v>1587</v>
+        <v>1595</v>
       </c>
       <c r="AH40" t="s">
         <v>42</v>
@@ -9253,7 +9337,7 @@
         <v>42</v>
       </c>
       <c r="AM40" t="s">
-        <v>1522</v>
+        <v>1530</v>
       </c>
       <c r="AN40" t="s">
         <v>42</v>
@@ -9291,25 +9375,25 @@
         <v>42</v>
       </c>
       <c r="Y41" t="s">
-        <v>1523</v>
+        <v>1531</v>
       </c>
       <c r="Z41" t="s">
         <v>42</v>
       </c>
       <c r="AA41" t="s">
-        <v>1523</v>
+        <v>1531</v>
       </c>
       <c r="AB41" t="s">
         <v>42</v>
       </c>
       <c r="AC41" t="s">
-        <v>1523</v>
+        <v>1531</v>
       </c>
       <c r="AD41" t="s">
         <v>42</v>
       </c>
       <c r="AG41" t="s">
-        <v>1588</v>
+        <v>1596</v>
       </c>
       <c r="AH41" t="s">
         <v>42</v>
@@ -9321,7 +9405,7 @@
         <v>42</v>
       </c>
       <c r="AM41" t="s">
-        <v>1523</v>
+        <v>1531</v>
       </c>
       <c r="AN41" t="s">
         <v>42</v>
@@ -9359,25 +9443,25 @@
         <v>42</v>
       </c>
       <c r="Y42" t="s">
-        <v>1524</v>
+        <v>1532</v>
       </c>
       <c r="Z42" t="s">
         <v>42</v>
       </c>
       <c r="AA42" t="s">
-        <v>1524</v>
+        <v>1532</v>
       </c>
       <c r="AB42" t="s">
         <v>42</v>
       </c>
       <c r="AC42" t="s">
-        <v>1524</v>
+        <v>1532</v>
       </c>
       <c r="AD42" t="s">
         <v>42</v>
       </c>
       <c r="AG42" t="s">
-        <v>1589</v>
+        <v>1597</v>
       </c>
       <c r="AH42" t="s">
         <v>42</v>
@@ -9389,7 +9473,7 @@
         <v>42</v>
       </c>
       <c r="AM42" t="s">
-        <v>1524</v>
+        <v>1532</v>
       </c>
       <c r="AN42" t="s">
         <v>42</v>
@@ -9427,25 +9511,25 @@
         <v>42</v>
       </c>
       <c r="Y43" t="s">
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="Z43" t="s">
         <v>42</v>
       </c>
       <c r="AA43" t="s">
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="AB43" t="s">
         <v>42</v>
       </c>
       <c r="AC43" t="s">
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="AD43" t="s">
         <v>42</v>
       </c>
       <c r="AG43" t="s">
-        <v>1590</v>
+        <v>1598</v>
       </c>
       <c r="AH43" t="s">
         <v>42</v>
@@ -9457,7 +9541,7 @@
         <v>42</v>
       </c>
       <c r="AM43" t="s">
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="AN43" t="s">
         <v>42</v>
@@ -9495,25 +9579,25 @@
         <v>42</v>
       </c>
       <c r="Y44" t="s">
-        <v>1526</v>
+        <v>1534</v>
       </c>
       <c r="Z44" t="s">
         <v>42</v>
       </c>
       <c r="AA44" t="s">
-        <v>1526</v>
+        <v>1534</v>
       </c>
       <c r="AB44" t="s">
         <v>42</v>
       </c>
       <c r="AC44" t="s">
-        <v>1526</v>
+        <v>1534</v>
       </c>
       <c r="AD44" t="s">
         <v>42</v>
       </c>
       <c r="AG44" t="s">
-        <v>1591</v>
+        <v>1599</v>
       </c>
       <c r="AH44" t="s">
         <v>42</v>
@@ -9525,7 +9609,7 @@
         <v>42</v>
       </c>
       <c r="AM44" t="s">
-        <v>1526</v>
+        <v>1534</v>
       </c>
       <c r="AN44" t="s">
         <v>42</v>
@@ -9563,25 +9647,25 @@
         <v>42</v>
       </c>
       <c r="Y45" t="s">
-        <v>1527</v>
+        <v>1535</v>
       </c>
       <c r="Z45" t="s">
         <v>42</v>
       </c>
       <c r="AA45" t="s">
-        <v>1527</v>
+        <v>1535</v>
       </c>
       <c r="AB45" t="s">
         <v>42</v>
       </c>
       <c r="AC45" t="s">
-        <v>1527</v>
+        <v>1535</v>
       </c>
       <c r="AD45" t="s">
         <v>42</v>
       </c>
       <c r="AG45" t="s">
-        <v>1592</v>
+        <v>1600</v>
       </c>
       <c r="AH45" t="s">
         <v>42</v>
@@ -9593,7 +9677,7 @@
         <v>42</v>
       </c>
       <c r="AM45" t="s">
-        <v>1527</v>
+        <v>1535</v>
       </c>
       <c r="AN45" t="s">
         <v>42</v>
@@ -9631,25 +9715,25 @@
         <v>42</v>
       </c>
       <c r="Y46" t="s">
-        <v>1528</v>
+        <v>1536</v>
       </c>
       <c r="Z46" t="s">
         <v>42</v>
       </c>
       <c r="AA46" t="s">
-        <v>1528</v>
+        <v>1536</v>
       </c>
       <c r="AB46" t="s">
         <v>42</v>
       </c>
       <c r="AC46" t="s">
-        <v>1528</v>
+        <v>1536</v>
       </c>
       <c r="AD46" t="s">
         <v>42</v>
       </c>
       <c r="AG46" t="s">
-        <v>1593</v>
+        <v>1601</v>
       </c>
       <c r="AH46" t="s">
         <v>42</v>
@@ -9661,7 +9745,7 @@
         <v>42</v>
       </c>
       <c r="AM46" t="s">
-        <v>1528</v>
+        <v>1536</v>
       </c>
       <c r="AN46" t="s">
         <v>42</v>
@@ -9699,25 +9783,25 @@
         <v>42</v>
       </c>
       <c r="Y47" t="s">
-        <v>1529</v>
+        <v>1537</v>
       </c>
       <c r="Z47" t="s">
         <v>42</v>
       </c>
       <c r="AA47" t="s">
-        <v>1529</v>
+        <v>1537</v>
       </c>
       <c r="AB47" t="s">
         <v>42</v>
       </c>
       <c r="AC47" t="s">
-        <v>1529</v>
+        <v>1537</v>
       </c>
       <c r="AD47" t="s">
         <v>42</v>
       </c>
       <c r="AG47" t="s">
-        <v>1594</v>
+        <v>1602</v>
       </c>
       <c r="AH47" t="s">
         <v>42</v>
@@ -9729,7 +9813,7 @@
         <v>42</v>
       </c>
       <c r="AM47" t="s">
-        <v>1529</v>
+        <v>1537</v>
       </c>
       <c r="AN47" t="s">
         <v>42</v>
@@ -9767,25 +9851,25 @@
         <v>42</v>
       </c>
       <c r="Y48" t="s">
-        <v>1530</v>
+        <v>1538</v>
       </c>
       <c r="Z48" t="s">
         <v>42</v>
       </c>
       <c r="AA48" t="s">
-        <v>1530</v>
+        <v>1538</v>
       </c>
       <c r="AB48" t="s">
         <v>42</v>
       </c>
       <c r="AC48" t="s">
-        <v>1530</v>
+        <v>1538</v>
       </c>
       <c r="AD48" t="s">
         <v>42</v>
       </c>
       <c r="AG48" t="s">
-        <v>1595</v>
+        <v>1603</v>
       </c>
       <c r="AH48" t="s">
         <v>42</v>
@@ -9797,7 +9881,7 @@
         <v>42</v>
       </c>
       <c r="AM48" t="s">
-        <v>1530</v>
+        <v>1538</v>
       </c>
       <c r="AN48" t="s">
         <v>42</v>
@@ -9835,25 +9919,25 @@
         <v>42</v>
       </c>
       <c r="Y49" t="s">
-        <v>1531</v>
+        <v>1539</v>
       </c>
       <c r="Z49" t="s">
         <v>42</v>
       </c>
       <c r="AA49" t="s">
-        <v>1531</v>
+        <v>1539</v>
       </c>
       <c r="AB49" t="s">
         <v>42</v>
       </c>
       <c r="AC49" t="s">
-        <v>1531</v>
+        <v>1539</v>
       </c>
       <c r="AD49" t="s">
         <v>42</v>
       </c>
       <c r="AG49" t="s">
-        <v>1596</v>
+        <v>1604</v>
       </c>
       <c r="AH49" t="s">
         <v>42</v>
@@ -9865,7 +9949,7 @@
         <v>42</v>
       </c>
       <c r="AM49" t="s">
-        <v>1531</v>
+        <v>1539</v>
       </c>
       <c r="AN49" t="s">
         <v>42</v>
@@ -9903,25 +9987,25 @@
         <v>42</v>
       </c>
       <c r="Y50" t="s">
-        <v>1532</v>
+        <v>1540</v>
       </c>
       <c r="Z50" t="s">
         <v>42</v>
       </c>
       <c r="AA50" t="s">
-        <v>1532</v>
+        <v>1540</v>
       </c>
       <c r="AB50" t="s">
         <v>42</v>
       </c>
       <c r="AC50" t="s">
-        <v>1532</v>
+        <v>1540</v>
       </c>
       <c r="AD50" t="s">
         <v>42</v>
       </c>
       <c r="AG50" t="s">
-        <v>1597</v>
+        <v>1605</v>
       </c>
       <c r="AH50" t="s">
         <v>42</v>
@@ -9933,7 +10017,7 @@
         <v>42</v>
       </c>
       <c r="AM50" t="s">
-        <v>1532</v>
+        <v>1540</v>
       </c>
       <c r="AN50" t="s">
         <v>42</v>
@@ -9971,25 +10055,25 @@
         <v>42</v>
       </c>
       <c r="Y51" t="s">
-        <v>1533</v>
+        <v>1541</v>
       </c>
       <c r="Z51" t="s">
         <v>42</v>
       </c>
       <c r="AA51" t="s">
-        <v>1533</v>
+        <v>1541</v>
       </c>
       <c r="AB51" t="s">
         <v>42</v>
       </c>
       <c r="AC51" t="s">
-        <v>1533</v>
+        <v>1541</v>
       </c>
       <c r="AD51" t="s">
         <v>42</v>
       </c>
       <c r="AG51" t="s">
-        <v>1598</v>
+        <v>1606</v>
       </c>
       <c r="AH51" t="s">
         <v>42</v>
@@ -10001,7 +10085,7 @@
         <v>42</v>
       </c>
       <c r="AM51" t="s">
-        <v>1533</v>
+        <v>1541</v>
       </c>
       <c r="AN51" t="s">
         <v>42</v>
@@ -10039,25 +10123,25 @@
         <v>42</v>
       </c>
       <c r="Y52" t="s">
-        <v>1534</v>
+        <v>1542</v>
       </c>
       <c r="Z52" t="s">
         <v>42</v>
       </c>
       <c r="AA52" t="s">
-        <v>1534</v>
+        <v>1542</v>
       </c>
       <c r="AB52" t="s">
         <v>42</v>
       </c>
       <c r="AC52" t="s">
-        <v>1534</v>
+        <v>1542</v>
       </c>
       <c r="AD52" t="s">
         <v>42</v>
       </c>
       <c r="AG52" t="s">
-        <v>1599</v>
+        <v>1607</v>
       </c>
       <c r="AH52" t="s">
         <v>42</v>
@@ -10069,7 +10153,7 @@
         <v>42</v>
       </c>
       <c r="AM52" t="s">
-        <v>1534</v>
+        <v>1542</v>
       </c>
       <c r="AN52" t="s">
         <v>42</v>
@@ -10107,25 +10191,25 @@
         <v>42</v>
       </c>
       <c r="Y53" t="s">
-        <v>1535</v>
+        <v>1543</v>
       </c>
       <c r="Z53" t="s">
         <v>42</v>
       </c>
       <c r="AA53" t="s">
-        <v>1535</v>
+        <v>1543</v>
       </c>
       <c r="AB53" t="s">
         <v>42</v>
       </c>
       <c r="AC53" t="s">
-        <v>1535</v>
+        <v>1543</v>
       </c>
       <c r="AD53" t="s">
         <v>42</v>
       </c>
       <c r="AG53" t="s">
-        <v>1600</v>
+        <v>1608</v>
       </c>
       <c r="AH53" t="s">
         <v>42</v>
@@ -10137,7 +10221,7 @@
         <v>42</v>
       </c>
       <c r="AM53" t="s">
-        <v>1535</v>
+        <v>1543</v>
       </c>
       <c r="AN53" t="s">
         <v>42</v>
@@ -10175,25 +10259,25 @@
         <v>42</v>
       </c>
       <c r="Y54" t="s">
-        <v>1536</v>
+        <v>1544</v>
       </c>
       <c r="Z54" t="s">
         <v>42</v>
       </c>
       <c r="AA54" t="s">
-        <v>1536</v>
+        <v>1544</v>
       </c>
       <c r="AB54" t="s">
         <v>42</v>
       </c>
       <c r="AC54" t="s">
-        <v>1536</v>
+        <v>1544</v>
       </c>
       <c r="AD54" t="s">
         <v>42</v>
       </c>
       <c r="AG54" t="s">
-        <v>1601</v>
+        <v>1609</v>
       </c>
       <c r="AH54" t="s">
         <v>42</v>
@@ -10205,7 +10289,7 @@
         <v>42</v>
       </c>
       <c r="AM54" t="s">
-        <v>1536</v>
+        <v>1544</v>
       </c>
       <c r="AN54" t="s">
         <v>42</v>
@@ -10243,25 +10327,25 @@
         <v>42</v>
       </c>
       <c r="Y55" t="s">
-        <v>1537</v>
+        <v>1545</v>
       </c>
       <c r="Z55" t="s">
         <v>42</v>
       </c>
       <c r="AA55" t="s">
-        <v>1537</v>
+        <v>1545</v>
       </c>
       <c r="AB55" t="s">
         <v>42</v>
       </c>
       <c r="AC55" t="s">
-        <v>1537</v>
+        <v>1545</v>
       </c>
       <c r="AD55" t="s">
         <v>42</v>
       </c>
       <c r="AG55" t="s">
-        <v>1602</v>
+        <v>1610</v>
       </c>
       <c r="AH55" t="s">
         <v>42</v>
@@ -10273,7 +10357,7 @@
         <v>42</v>
       </c>
       <c r="AM55" t="s">
-        <v>1537</v>
+        <v>1545</v>
       </c>
       <c r="AN55" t="s">
         <v>42</v>
@@ -10311,25 +10395,25 @@
         <v>42</v>
       </c>
       <c r="Y56" t="s">
-        <v>1538</v>
+        <v>1546</v>
       </c>
       <c r="Z56" t="s">
         <v>42</v>
       </c>
       <c r="AA56" t="s">
-        <v>1538</v>
+        <v>1546</v>
       </c>
       <c r="AB56" t="s">
         <v>42</v>
       </c>
       <c r="AC56" t="s">
-        <v>1538</v>
+        <v>1546</v>
       </c>
       <c r="AD56" t="s">
         <v>42</v>
       </c>
       <c r="AG56" t="s">
-        <v>1603</v>
+        <v>1611</v>
       </c>
       <c r="AH56" t="s">
         <v>42</v>
@@ -10341,7 +10425,7 @@
         <v>42</v>
       </c>
       <c r="AM56" t="s">
-        <v>1538</v>
+        <v>1546</v>
       </c>
       <c r="AN56" t="s">
         <v>42</v>
@@ -10379,25 +10463,25 @@
         <v>42</v>
       </c>
       <c r="Y57" t="s">
-        <v>1539</v>
+        <v>1547</v>
       </c>
       <c r="Z57" t="s">
         <v>42</v>
       </c>
       <c r="AA57" t="s">
-        <v>1539</v>
+        <v>1547</v>
       </c>
       <c r="AB57" t="s">
         <v>42</v>
       </c>
       <c r="AC57" t="s">
-        <v>1539</v>
+        <v>1547</v>
       </c>
       <c r="AD57" t="s">
         <v>42</v>
       </c>
       <c r="AG57" t="s">
-        <v>1604</v>
+        <v>1612</v>
       </c>
       <c r="AH57" t="s">
         <v>42</v>
@@ -10409,7 +10493,7 @@
         <v>42</v>
       </c>
       <c r="AM57" t="s">
-        <v>1539</v>
+        <v>1547</v>
       </c>
       <c r="AN57" t="s">
         <v>42</v>
@@ -10447,25 +10531,25 @@
         <v>42</v>
       </c>
       <c r="Y58" t="s">
-        <v>1540</v>
+        <v>1548</v>
       </c>
       <c r="Z58" t="s">
         <v>42</v>
       </c>
       <c r="AA58" t="s">
-        <v>1540</v>
+        <v>1548</v>
       </c>
       <c r="AB58" t="s">
         <v>42</v>
       </c>
       <c r="AC58" t="s">
-        <v>1540</v>
+        <v>1548</v>
       </c>
       <c r="AD58" t="s">
         <v>42</v>
       </c>
       <c r="AG58" t="s">
-        <v>1605</v>
+        <v>1613</v>
       </c>
       <c r="AH58" t="s">
         <v>42</v>
@@ -10477,7 +10561,7 @@
         <v>42</v>
       </c>
       <c r="AM58" t="s">
-        <v>1540</v>
+        <v>1548</v>
       </c>
       <c r="AN58" t="s">
         <v>42</v>
@@ -10515,25 +10599,25 @@
         <v>42</v>
       </c>
       <c r="Y59" t="s">
-        <v>1541</v>
+        <v>1549</v>
       </c>
       <c r="Z59" t="s">
         <v>42</v>
       </c>
       <c r="AA59" t="s">
-        <v>1541</v>
+        <v>1549</v>
       </c>
       <c r="AB59" t="s">
         <v>42</v>
       </c>
       <c r="AC59" t="s">
-        <v>1541</v>
+        <v>1549</v>
       </c>
       <c r="AD59" t="s">
         <v>42</v>
       </c>
       <c r="AG59" t="s">
-        <v>1606</v>
+        <v>1614</v>
       </c>
       <c r="AH59" t="s">
         <v>42</v>
@@ -10545,7 +10629,7 @@
         <v>42</v>
       </c>
       <c r="AM59" t="s">
-        <v>1541</v>
+        <v>1549</v>
       </c>
       <c r="AN59" t="s">
         <v>42</v>
@@ -10583,25 +10667,25 @@
         <v>42</v>
       </c>
       <c r="Y60" t="s">
-        <v>1542</v>
+        <v>1550</v>
       </c>
       <c r="Z60" t="s">
         <v>42</v>
       </c>
       <c r="AA60" t="s">
-        <v>1542</v>
+        <v>1550</v>
       </c>
       <c r="AB60" t="s">
         <v>42</v>
       </c>
       <c r="AC60" t="s">
-        <v>1542</v>
+        <v>1550</v>
       </c>
       <c r="AD60" t="s">
         <v>42</v>
       </c>
       <c r="AG60" t="s">
-        <v>1535</v>
+        <v>1543</v>
       </c>
       <c r="AH60" t="s">
         <v>42</v>
@@ -10613,7 +10697,7 @@
         <v>42</v>
       </c>
       <c r="AM60" t="s">
-        <v>1542</v>
+        <v>1550</v>
       </c>
       <c r="AN60" t="s">
         <v>42</v>
@@ -10651,25 +10735,25 @@
         <v>42</v>
       </c>
       <c r="Y61" t="s">
-        <v>1543</v>
+        <v>1551</v>
       </c>
       <c r="Z61" t="s">
         <v>42</v>
       </c>
       <c r="AA61" t="s">
-        <v>1543</v>
+        <v>1551</v>
       </c>
       <c r="AB61" t="s">
         <v>42</v>
       </c>
       <c r="AC61" t="s">
-        <v>1543</v>
+        <v>1551</v>
       </c>
       <c r="AD61" t="s">
         <v>42</v>
       </c>
       <c r="AG61" t="s">
-        <v>1607</v>
+        <v>1615</v>
       </c>
       <c r="AH61" t="s">
         <v>42</v>
@@ -10681,7 +10765,7 @@
         <v>42</v>
       </c>
       <c r="AM61" t="s">
-        <v>1543</v>
+        <v>1551</v>
       </c>
       <c r="AN61" t="s">
         <v>42</v>
@@ -10719,25 +10803,25 @@
         <v>42</v>
       </c>
       <c r="Y62" t="s">
-        <v>1544</v>
+        <v>1552</v>
       </c>
       <c r="Z62" t="s">
         <v>42</v>
       </c>
       <c r="AA62" t="s">
-        <v>1544</v>
+        <v>1552</v>
       </c>
       <c r="AB62" t="s">
         <v>42</v>
       </c>
       <c r="AC62" t="s">
-        <v>1544</v>
+        <v>1552</v>
       </c>
       <c r="AD62" t="s">
         <v>42</v>
       </c>
       <c r="AG62" t="s">
-        <v>1608</v>
+        <v>1616</v>
       </c>
       <c r="AH62" t="s">
         <v>42</v>
@@ -10749,7 +10833,7 @@
         <v>42</v>
       </c>
       <c r="AM62" t="s">
-        <v>1544</v>
+        <v>1552</v>
       </c>
       <c r="AN62" t="s">
         <v>42</v>
@@ -10787,25 +10871,25 @@
         <v>42</v>
       </c>
       <c r="Y63" t="s">
-        <v>1545</v>
+        <v>1553</v>
       </c>
       <c r="Z63" t="s">
         <v>42</v>
       </c>
       <c r="AA63" t="s">
-        <v>1545</v>
+        <v>1553</v>
       </c>
       <c r="AB63" t="s">
         <v>42</v>
       </c>
       <c r="AC63" t="s">
-        <v>1545</v>
+        <v>1553</v>
       </c>
       <c r="AD63" t="s">
         <v>42</v>
       </c>
       <c r="AG63" t="s">
-        <v>1609</v>
+        <v>1617</v>
       </c>
       <c r="AH63" t="s">
         <v>42</v>
@@ -10817,7 +10901,7 @@
         <v>42</v>
       </c>
       <c r="AM63" t="s">
-        <v>1545</v>
+        <v>1553</v>
       </c>
       <c r="AN63" t="s">
         <v>42</v>
@@ -10873,7 +10957,7 @@
         <v>42</v>
       </c>
       <c r="AG64" t="s">
-        <v>1610</v>
+        <v>1618</v>
       </c>
       <c r="AH64" t="s">
         <v>42</v>
@@ -10923,25 +11007,25 @@
         <v>42</v>
       </c>
       <c r="Y65" t="s">
-        <v>1546</v>
+        <v>1554</v>
       </c>
       <c r="Z65" t="s">
         <v>42</v>
       </c>
       <c r="AA65" t="s">
-        <v>1546</v>
+        <v>1554</v>
       </c>
       <c r="AB65" t="s">
         <v>42</v>
       </c>
       <c r="AC65" t="s">
-        <v>1546</v>
+        <v>1554</v>
       </c>
       <c r="AD65" t="s">
         <v>42</v>
       </c>
       <c r="AG65" t="s">
-        <v>1611</v>
+        <v>1619</v>
       </c>
       <c r="AH65" t="s">
         <v>42</v>
@@ -10953,7 +11037,7 @@
         <v>42</v>
       </c>
       <c r="AM65" t="s">
-        <v>1546</v>
+        <v>1554</v>
       </c>
       <c r="AN65" t="s">
         <v>42</v>
@@ -10991,25 +11075,25 @@
         <v>42</v>
       </c>
       <c r="Y66" t="s">
-        <v>1547</v>
+        <v>1555</v>
       </c>
       <c r="Z66" t="s">
         <v>42</v>
       </c>
       <c r="AA66" t="s">
-        <v>1547</v>
+        <v>1555</v>
       </c>
       <c r="AB66" t="s">
         <v>42</v>
       </c>
       <c r="AC66" t="s">
-        <v>1547</v>
+        <v>1555</v>
       </c>
       <c r="AD66" t="s">
         <v>42</v>
       </c>
       <c r="AG66" t="s">
-        <v>1612</v>
+        <v>1620</v>
       </c>
       <c r="AH66" t="s">
         <v>42</v>
@@ -11021,7 +11105,7 @@
         <v>42</v>
       </c>
       <c r="AM66" t="s">
-        <v>1547</v>
+        <v>1555</v>
       </c>
       <c r="AN66" t="s">
         <v>42</v>
@@ -11059,25 +11143,25 @@
         <v>42</v>
       </c>
       <c r="Y67" t="s">
-        <v>1548</v>
+        <v>1556</v>
       </c>
       <c r="Z67" t="s">
         <v>42</v>
       </c>
       <c r="AA67" t="s">
-        <v>1548</v>
+        <v>1556</v>
       </c>
       <c r="AB67" t="s">
         <v>42</v>
       </c>
       <c r="AC67" t="s">
-        <v>1548</v>
+        <v>1556</v>
       </c>
       <c r="AD67" t="s">
         <v>42</v>
       </c>
       <c r="AG67" t="s">
-        <v>1613</v>
+        <v>1621</v>
       </c>
       <c r="AH67" t="s">
         <v>42</v>
@@ -11089,7 +11173,7 @@
         <v>42</v>
       </c>
       <c r="AM67" t="s">
-        <v>1548</v>
+        <v>1556</v>
       </c>
       <c r="AN67" t="s">
         <v>42</v>
@@ -11127,25 +11211,25 @@
         <v>42</v>
       </c>
       <c r="Y68" t="s">
-        <v>1549</v>
+        <v>1557</v>
       </c>
       <c r="Z68" t="s">
         <v>42</v>
       </c>
       <c r="AA68" t="s">
-        <v>1549</v>
+        <v>1557</v>
       </c>
       <c r="AB68" t="s">
         <v>42</v>
       </c>
       <c r="AC68" t="s">
-        <v>1549</v>
+        <v>1557</v>
       </c>
       <c r="AD68" t="s">
         <v>42</v>
       </c>
       <c r="AG68" t="s">
-        <v>1614</v>
+        <v>1622</v>
       </c>
       <c r="AH68" t="s">
         <v>42</v>
@@ -11157,7 +11241,7 @@
         <v>42</v>
       </c>
       <c r="AM68" t="s">
-        <v>1549</v>
+        <v>1557</v>
       </c>
       <c r="AN68" t="s">
         <v>42</v>
@@ -11195,7 +11279,7 @@
         <v>42</v>
       </c>
       <c r="AG69" t="s">
-        <v>1615</v>
+        <v>1623</v>
       </c>
       <c r="AH69" t="s">
         <v>42</v>
@@ -11239,7 +11323,7 @@
         <v>42</v>
       </c>
       <c r="AG70" t="s">
-        <v>1616</v>
+        <v>1624</v>
       </c>
       <c r="AH70" t="s">
         <v>42</v>
@@ -11283,7 +11367,7 @@
         <v>42</v>
       </c>
       <c r="AG71" t="s">
-        <v>1617</v>
+        <v>1625</v>
       </c>
       <c r="AH71" t="s">
         <v>42</v>
@@ -11327,7 +11411,7 @@
         <v>42</v>
       </c>
       <c r="AG72" t="s">
-        <v>1618</v>
+        <v>1626</v>
       </c>
       <c r="AH72" t="s">
         <v>42</v>
@@ -11371,7 +11455,7 @@
         <v>42</v>
       </c>
       <c r="AG73" t="s">
-        <v>1619</v>
+        <v>1627</v>
       </c>
       <c r="AH73" t="s">
         <v>42</v>
@@ -11415,7 +11499,7 @@
         <v>42</v>
       </c>
       <c r="AG74" t="s">
-        <v>1620</v>
+        <v>1628</v>
       </c>
       <c r="AH74" t="s">
         <v>42</v>
@@ -11459,7 +11543,7 @@
         <v>42</v>
       </c>
       <c r="AG75" t="s">
-        <v>1621</v>
+        <v>1629</v>
       </c>
       <c r="AH75" t="s">
         <v>42</v>
@@ -11503,7 +11587,7 @@
         <v>42</v>
       </c>
       <c r="AG76" t="s">
-        <v>1622</v>
+        <v>1630</v>
       </c>
       <c r="AH76" t="s">
         <v>42</v>
@@ -11547,7 +11631,7 @@
         <v>42</v>
       </c>
       <c r="AG77" t="s">
-        <v>1623</v>
+        <v>1631</v>
       </c>
       <c r="AH77" t="s">
         <v>42</v>
@@ -11591,7 +11675,7 @@
         <v>42</v>
       </c>
       <c r="AG78" t="s">
-        <v>1624</v>
+        <v>1632</v>
       </c>
       <c r="AH78" t="s">
         <v>42</v>
@@ -11635,7 +11719,7 @@
         <v>42</v>
       </c>
       <c r="AG79" t="s">
-        <v>1625</v>
+        <v>1633</v>
       </c>
       <c r="AH79" t="s">
         <v>42</v>
@@ -11679,7 +11763,7 @@
         <v>42</v>
       </c>
       <c r="AG80" t="s">
-        <v>1626</v>
+        <v>1634</v>
       </c>
       <c r="AH80" t="s">
         <v>42</v>
@@ -11723,7 +11807,7 @@
         <v>42</v>
       </c>
       <c r="AG81" t="s">
-        <v>1627</v>
+        <v>1635</v>
       </c>
       <c r="AH81" t="s">
         <v>42</v>
@@ -11767,7 +11851,7 @@
         <v>42</v>
       </c>
       <c r="AG82" t="s">
-        <v>1628</v>
+        <v>1636</v>
       </c>
       <c r="AH82" t="s">
         <v>42</v>
@@ -11811,7 +11895,7 @@
         <v>42</v>
       </c>
       <c r="AG83" t="s">
-        <v>1629</v>
+        <v>1637</v>
       </c>
       <c r="AH83" t="s">
         <v>42</v>
@@ -11855,7 +11939,7 @@
         <v>42</v>
       </c>
       <c r="AG84" t="s">
-        <v>1630</v>
+        <v>1638</v>
       </c>
       <c r="AH84" t="s">
         <v>42</v>
@@ -11899,7 +11983,7 @@
         <v>42</v>
       </c>
       <c r="AG85" t="s">
-        <v>1631</v>
+        <v>1639</v>
       </c>
       <c r="AH85" t="s">
         <v>42</v>
@@ -11943,7 +12027,7 @@
         <v>42</v>
       </c>
       <c r="AG86" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
       <c r="AH86" t="s">
         <v>42</v>
@@ -11969,7 +12053,7 @@
         <v>42</v>
       </c>
       <c r="AG87" t="s">
-        <v>1633</v>
+        <v>1641</v>
       </c>
       <c r="AH87" t="s">
         <v>42</v>
@@ -11989,7 +12073,7 @@
         <v>42</v>
       </c>
       <c r="AG88" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
       <c r="AH88" t="s">
         <v>42</v>
@@ -12009,7 +12093,7 @@
         <v>42</v>
       </c>
       <c r="AG89" t="s">
-        <v>1635</v>
+        <v>1643</v>
       </c>
       <c r="AH89" t="s">
         <v>42</v>
@@ -12029,7 +12113,7 @@
         <v>42</v>
       </c>
       <c r="AG90" t="s">
-        <v>1636</v>
+        <v>1644</v>
       </c>
       <c r="AH90" t="s">
         <v>42</v>
@@ -12049,7 +12133,7 @@
         <v>42</v>
       </c>
       <c r="AG91" t="s">
-        <v>1637</v>
+        <v>1645</v>
       </c>
       <c r="AH91" t="s">
         <v>42</v>
@@ -12089,7 +12173,7 @@
         <v>42</v>
       </c>
       <c r="AG93" t="s">
-        <v>1638</v>
+        <v>1646</v>
       </c>
       <c r="AH93" t="s">
         <v>42</v>
@@ -12109,7 +12193,7 @@
         <v>42</v>
       </c>
       <c r="AG94" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
       <c r="AH94" t="s">
         <v>42</v>
@@ -12129,7 +12213,7 @@
         <v>42</v>
       </c>
       <c r="AG95" t="s">
-        <v>1640</v>
+        <v>1648</v>
       </c>
       <c r="AH95" t="s">
         <v>42</v>
@@ -12149,7 +12233,7 @@
         <v>42</v>
       </c>
       <c r="AG96" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
       <c r="AH96" t="s">
         <v>42</v>
@@ -12169,7 +12253,7 @@
         <v>42</v>
       </c>
       <c r="AG97" t="s">
-        <v>1642</v>
+        <v>1650</v>
       </c>
       <c r="AH97" t="s">
         <v>42</v>
@@ -12189,7 +12273,7 @@
         <v>42</v>
       </c>
       <c r="AG98" t="s">
-        <v>1643</v>
+        <v>1651</v>
       </c>
       <c r="AH98" t="s">
         <v>42</v>
@@ -12209,7 +12293,7 @@
         <v>42</v>
       </c>
       <c r="AG99" t="s">
-        <v>1644</v>
+        <v>1652</v>
       </c>
       <c r="AH99" t="s">
         <v>42</v>
@@ -12229,7 +12313,7 @@
         <v>42</v>
       </c>
       <c r="AG100" t="s">
-        <v>1645</v>
+        <v>1653</v>
       </c>
       <c r="AH100" t="s">
         <v>42</v>
@@ -12249,7 +12333,7 @@
         <v>42</v>
       </c>
       <c r="AG101" t="s">
-        <v>1646</v>
+        <v>1654</v>
       </c>
       <c r="AH101" t="s">
         <v>42</v>
@@ -12269,7 +12353,7 @@
         <v>42</v>
       </c>
       <c r="AG102" t="s">
-        <v>1647</v>
+        <v>1655</v>
       </c>
       <c r="AH102" t="s">
         <v>42</v>
@@ -12289,7 +12373,7 @@
         <v>42</v>
       </c>
       <c r="AG103" t="s">
-        <v>1648</v>
+        <v>1656</v>
       </c>
       <c r="AH103" t="s">
         <v>42</v>
@@ -12309,7 +12393,7 @@
         <v>42</v>
       </c>
       <c r="AG104" t="s">
-        <v>1649</v>
+        <v>1657</v>
       </c>
       <c r="AH104" t="s">
         <v>42</v>
@@ -12329,7 +12413,7 @@
         <v>42</v>
       </c>
       <c r="AG105" t="s">
-        <v>1650</v>
+        <v>1658</v>
       </c>
       <c r="AH105" t="s">
         <v>42</v>
@@ -12349,7 +12433,7 @@
         <v>42</v>
       </c>
       <c r="AG106" t="s">
-        <v>1651</v>
+        <v>1659</v>
       </c>
       <c r="AH106" t="s">
         <v>42</v>
@@ -12369,7 +12453,7 @@
         <v>42</v>
       </c>
       <c r="AG107" t="s">
-        <v>1652</v>
+        <v>1660</v>
       </c>
       <c r="AH107" t="s">
         <v>42</v>
@@ -12389,7 +12473,7 @@
         <v>42</v>
       </c>
       <c r="AG108" t="s">
-        <v>1653</v>
+        <v>1661</v>
       </c>
       <c r="AH108" t="s">
         <v>42</v>
@@ -12409,7 +12493,7 @@
         <v>42</v>
       </c>
       <c r="AG109" t="s">
-        <v>1654</v>
+        <v>1662</v>
       </c>
       <c r="AH109" t="s">
         <v>42</v>
@@ -12429,7 +12513,7 @@
         <v>42</v>
       </c>
       <c r="AG110" t="s">
-        <v>1655</v>
+        <v>1663</v>
       </c>
       <c r="AH110" t="s">
         <v>42</v>
@@ -12449,7 +12533,7 @@
         <v>42</v>
       </c>
       <c r="AG111" t="s">
-        <v>1656</v>
+        <v>1664</v>
       </c>
       <c r="AH111" t="s">
         <v>42</v>
@@ -12469,7 +12553,7 @@
         <v>42</v>
       </c>
       <c r="AG112" t="s">
-        <v>1657</v>
+        <v>1665</v>
       </c>
       <c r="AH112" t="s">
         <v>42</v>
@@ -12489,7 +12573,7 @@
         <v>42</v>
       </c>
       <c r="AG113" t="s">
-        <v>1658</v>
+        <v>1666</v>
       </c>
       <c r="AH113" t="s">
         <v>42</v>
@@ -12509,7 +12593,7 @@
         <v>42</v>
       </c>
       <c r="AG114" t="s">
-        <v>1659</v>
+        <v>1667</v>
       </c>
       <c r="AH114" t="s">
         <v>42</v>
@@ -12529,7 +12613,7 @@
         <v>42</v>
       </c>
       <c r="AG115" t="s">
-        <v>1660</v>
+        <v>1668</v>
       </c>
       <c r="AH115" t="s">
         <v>42</v>
@@ -12549,7 +12633,7 @@
         <v>42</v>
       </c>
       <c r="AG116" t="s">
-        <v>1661</v>
+        <v>1669</v>
       </c>
       <c r="AH116" t="s">
         <v>42</v>
@@ -12569,7 +12653,7 @@
         <v>42</v>
       </c>
       <c r="AG117" t="s">
-        <v>1662</v>
+        <v>1670</v>
       </c>
       <c r="AH117" t="s">
         <v>42</v>
@@ -12589,7 +12673,7 @@
         <v>42</v>
       </c>
       <c r="AG118" t="s">
-        <v>1663</v>
+        <v>1671</v>
       </c>
       <c r="AH118" t="s">
         <v>42</v>
@@ -12609,7 +12693,7 @@
         <v>42</v>
       </c>
       <c r="AG119" t="s">
-        <v>1664</v>
+        <v>1672</v>
       </c>
       <c r="AH119" t="s">
         <v>42</v>
@@ -12629,7 +12713,7 @@
         <v>42</v>
       </c>
       <c r="AG120" t="s">
-        <v>1665</v>
+        <v>1673</v>
       </c>
       <c r="AH120" t="s">
         <v>42</v>
@@ -12649,7 +12733,7 @@
         <v>42</v>
       </c>
       <c r="AG121" t="s">
-        <v>1666</v>
+        <v>1674</v>
       </c>
       <c r="AH121" t="s">
         <v>42</v>
@@ -12669,7 +12753,7 @@
         <v>42</v>
       </c>
       <c r="AG122" t="s">
-        <v>1667</v>
+        <v>1675</v>
       </c>
       <c r="AH122" t="s">
         <v>42</v>
@@ -12689,7 +12773,7 @@
         <v>42</v>
       </c>
       <c r="AG123" t="s">
-        <v>1668</v>
+        <v>1676</v>
       </c>
       <c r="AH123" t="s">
         <v>42</v>
@@ -12709,7 +12793,7 @@
         <v>42</v>
       </c>
       <c r="AG124" t="s">
-        <v>1669</v>
+        <v>1677</v>
       </c>
       <c r="AH124" t="s">
         <v>42</v>
@@ -12729,7 +12813,7 @@
         <v>42</v>
       </c>
       <c r="AG125" t="s">
-        <v>1670</v>
+        <v>1678</v>
       </c>
       <c r="AH125" t="s">
         <v>42</v>
@@ -12749,7 +12833,7 @@
         <v>42</v>
       </c>
       <c r="AG126" t="s">
-        <v>1671</v>
+        <v>1679</v>
       </c>
       <c r="AH126" t="s">
         <v>42</v>
@@ -12769,7 +12853,7 @@
         <v>42</v>
       </c>
       <c r="AG127" t="s">
-        <v>1672</v>
+        <v>1680</v>
       </c>
       <c r="AH127" t="s">
         <v>42</v>
@@ -12789,7 +12873,7 @@
         <v>42</v>
       </c>
       <c r="AG128" t="s">
-        <v>1673</v>
+        <v>1681</v>
       </c>
       <c r="AH128" t="s">
         <v>42</v>
@@ -12809,7 +12893,7 @@
         <v>42</v>
       </c>
       <c r="AG129" t="s">
-        <v>1674</v>
+        <v>1682</v>
       </c>
       <c r="AH129" t="s">
         <v>42</v>
@@ -12829,7 +12913,7 @@
         <v>42</v>
       </c>
       <c r="AG130" t="s">
-        <v>1675</v>
+        <v>1683</v>
       </c>
       <c r="AH130" t="s">
         <v>42</v>
@@ -12849,7 +12933,7 @@
         <v>42</v>
       </c>
       <c r="AG131" t="s">
-        <v>1676</v>
+        <v>1684</v>
       </c>
       <c r="AH131" t="s">
         <v>42</v>
@@ -12869,7 +12953,7 @@
         <v>42</v>
       </c>
       <c r="AG132" t="s">
-        <v>1677</v>
+        <v>1685</v>
       </c>
       <c r="AH132" t="s">
         <v>42</v>
@@ -12889,7 +12973,7 @@
         <v>42</v>
       </c>
       <c r="AG133" t="s">
-        <v>1678</v>
+        <v>1686</v>
       </c>
       <c r="AH133" t="s">
         <v>42</v>
@@ -12909,7 +12993,7 @@
         <v>42</v>
       </c>
       <c r="AG134" t="s">
-        <v>1679</v>
+        <v>1687</v>
       </c>
       <c r="AH134" t="s">
         <v>42</v>
@@ -12929,7 +13013,7 @@
         <v>42</v>
       </c>
       <c r="AG135" t="s">
-        <v>1680</v>
+        <v>1688</v>
       </c>
       <c r="AH135" t="s">
         <v>42</v>
@@ -12949,7 +13033,7 @@
         <v>42</v>
       </c>
       <c r="AG136" t="s">
-        <v>1681</v>
+        <v>1689</v>
       </c>
       <c r="AH136" t="s">
         <v>42</v>
@@ -12969,7 +13053,7 @@
         <v>42</v>
       </c>
       <c r="AG137" t="s">
-        <v>1682</v>
+        <v>1690</v>
       </c>
       <c r="AH137" t="s">
         <v>42</v>
@@ -12989,7 +13073,7 @@
         <v>42</v>
       </c>
       <c r="AG138" t="s">
-        <v>1683</v>
+        <v>1691</v>
       </c>
       <c r="AH138" t="s">
         <v>42</v>
@@ -13009,7 +13093,7 @@
         <v>42</v>
       </c>
       <c r="AG139" t="s">
-        <v>1684</v>
+        <v>1692</v>
       </c>
       <c r="AH139" t="s">
         <v>42</v>
@@ -13029,7 +13113,7 @@
         <v>42</v>
       </c>
       <c r="AG140" t="s">
-        <v>1685</v>
+        <v>1693</v>
       </c>
       <c r="AH140" t="s">
         <v>42</v>
@@ -13049,7 +13133,7 @@
         <v>42</v>
       </c>
       <c r="AG141" t="s">
-        <v>1686</v>
+        <v>1694</v>
       </c>
       <c r="AH141" t="s">
         <v>42</v>
@@ -13089,7 +13173,7 @@
         <v>42</v>
       </c>
       <c r="AG143" t="s">
-        <v>1687</v>
+        <v>1695</v>
       </c>
       <c r="AH143" t="s">
         <v>42</v>
@@ -13109,7 +13193,7 @@
         <v>42</v>
       </c>
       <c r="AG144" t="s">
-        <v>1688</v>
+        <v>1696</v>
       </c>
       <c r="AH144" t="s">
         <v>42</v>
@@ -13129,7 +13213,7 @@
         <v>42</v>
       </c>
       <c r="AG145" t="s">
-        <v>1689</v>
+        <v>1697</v>
       </c>
       <c r="AH145" t="s">
         <v>42</v>
@@ -13149,7 +13233,7 @@
         <v>42</v>
       </c>
       <c r="AG146" t="s">
-        <v>1690</v>
+        <v>1698</v>
       </c>
       <c r="AH146" t="s">
         <v>42</v>
@@ -13169,7 +13253,7 @@
         <v>42</v>
       </c>
       <c r="AG147" t="s">
-        <v>1691</v>
+        <v>1699</v>
       </c>
       <c r="AH147" t="s">
         <v>42</v>
@@ -13189,7 +13273,7 @@
         <v>42</v>
       </c>
       <c r="AG148" t="s">
-        <v>1692</v>
+        <v>1700</v>
       </c>
       <c r="AH148" t="s">
         <v>42</v>
@@ -13209,7 +13293,7 @@
         <v>42</v>
       </c>
       <c r="AG149" t="s">
-        <v>1693</v>
+        <v>1701</v>
       </c>
       <c r="AH149" t="s">
         <v>42</v>
@@ -13229,7 +13313,7 @@
         <v>42</v>
       </c>
       <c r="AG150" t="s">
-        <v>1694</v>
+        <v>1702</v>
       </c>
       <c r="AH150" t="s">
         <v>42</v>
@@ -13249,7 +13333,7 @@
         <v>42</v>
       </c>
       <c r="AG151" t="s">
-        <v>1695</v>
+        <v>1703</v>
       </c>
       <c r="AH151" t="s">
         <v>42</v>
@@ -13269,7 +13353,7 @@
         <v>42</v>
       </c>
       <c r="AG152" t="s">
-        <v>1696</v>
+        <v>1704</v>
       </c>
       <c r="AH152" t="s">
         <v>42</v>
@@ -13289,7 +13373,7 @@
         <v>42</v>
       </c>
       <c r="AG153" t="s">
-        <v>1697</v>
+        <v>1705</v>
       </c>
       <c r="AH153" t="s">
         <v>42</v>
@@ -13309,7 +13393,7 @@
         <v>42</v>
       </c>
       <c r="AG154" t="s">
-        <v>1698</v>
+        <v>1706</v>
       </c>
       <c r="AH154" t="s">
         <v>42</v>
@@ -13329,7 +13413,7 @@
         <v>42</v>
       </c>
       <c r="AG155" t="s">
-        <v>1699</v>
+        <v>1707</v>
       </c>
       <c r="AH155" t="s">
         <v>42</v>
@@ -13349,7 +13433,7 @@
         <v>42</v>
       </c>
       <c r="AG156" t="s">
-        <v>1700</v>
+        <v>1708</v>
       </c>
       <c r="AH156" t="s">
         <v>42</v>
@@ -13369,7 +13453,7 @@
         <v>42</v>
       </c>
       <c r="AG157" t="s">
-        <v>1701</v>
+        <v>1709</v>
       </c>
       <c r="AH157" t="s">
         <v>42</v>
@@ -13389,7 +13473,7 @@
         <v>42</v>
       </c>
       <c r="AG158" t="s">
-        <v>1702</v>
+        <v>1710</v>
       </c>
       <c r="AH158" t="s">
         <v>42</v>
@@ -13409,7 +13493,7 @@
         <v>42</v>
       </c>
       <c r="AG159" t="s">
-        <v>1703</v>
+        <v>1711</v>
       </c>
       <c r="AH159" t="s">
         <v>42</v>
@@ -13429,7 +13513,7 @@
         <v>42</v>
       </c>
       <c r="AG160" t="s">
-        <v>1704</v>
+        <v>1712</v>
       </c>
       <c r="AH160" t="s">
         <v>42</v>
@@ -13449,7 +13533,7 @@
         <v>42</v>
       </c>
       <c r="AG161" t="s">
-        <v>1705</v>
+        <v>1713</v>
       </c>
       <c r="AH161" t="s">
         <v>42</v>
@@ -13468,6 +13552,12 @@
       <c r="X162" t="s">
         <v>42</v>
       </c>
+      <c r="AG162" t="s">
+        <v>1714</v>
+      </c>
+      <c r="AH162" t="s">
+        <v>42</v>
+      </c>
       <c r="AK162" t="s">
         <v>654</v>
       </c>
@@ -13482,6 +13572,12 @@
       <c r="X163" t="s">
         <v>42</v>
       </c>
+      <c r="AG163" t="s">
+        <v>1715</v>
+      </c>
+      <c r="AH163" t="s">
+        <v>42</v>
+      </c>
       <c r="AK163" t="s">
         <v>655</v>
       </c>
@@ -13496,6 +13592,12 @@
       <c r="X164" t="s">
         <v>42</v>
       </c>
+      <c r="AG164" t="s">
+        <v>1716</v>
+      </c>
+      <c r="AH164" t="s">
+        <v>42</v>
+      </c>
       <c r="AK164" t="s">
         <v>656</v>
       </c>
@@ -13510,6 +13612,12 @@
       <c r="X165" t="s">
         <v>42</v>
       </c>
+      <c r="AG165" t="s">
+        <v>1717</v>
+      </c>
+      <c r="AH165" t="s">
+        <v>42</v>
+      </c>
       <c r="AK165" t="s">
         <v>657</v>
       </c>
@@ -13524,6 +13632,12 @@
       <c r="X166" t="s">
         <v>42</v>
       </c>
+      <c r="AG166" t="s">
+        <v>1718</v>
+      </c>
+      <c r="AH166" t="s">
+        <v>42</v>
+      </c>
       <c r="AK166" t="s">
         <v>658</v>
       </c>
@@ -13538,6 +13652,12 @@
       <c r="X167" t="s">
         <v>42</v>
       </c>
+      <c r="AG167" t="s">
+        <v>1719</v>
+      </c>
+      <c r="AH167" t="s">
+        <v>42</v>
+      </c>
       <c r="AK167" t="s">
         <v>659</v>
       </c>
@@ -13552,6 +13672,12 @@
       <c r="X168" t="s">
         <v>42</v>
       </c>
+      <c r="AG168" t="s">
+        <v>1720</v>
+      </c>
+      <c r="AH168" t="s">
+        <v>42</v>
+      </c>
       <c r="AK168" t="s">
         <v>660</v>
       </c>
@@ -13566,6 +13692,12 @@
       <c r="X169" t="s">
         <v>42</v>
       </c>
+      <c r="AG169" t="s">
+        <v>1721</v>
+      </c>
+      <c r="AH169" t="s">
+        <v>42</v>
+      </c>
       <c r="AK169" t="s">
         <v>661</v>
       </c>
@@ -13580,6 +13712,12 @@
       <c r="X170" t="s">
         <v>42</v>
       </c>
+      <c r="AG170" t="s">
+        <v>1722</v>
+      </c>
+      <c r="AH170" t="s">
+        <v>42</v>
+      </c>
       <c r="AK170" t="s">
         <v>662</v>
       </c>
@@ -13594,6 +13732,12 @@
       <c r="X171" t="s">
         <v>42</v>
       </c>
+      <c r="AG171" t="s">
+        <v>1723</v>
+      </c>
+      <c r="AH171" t="s">
+        <v>42</v>
+      </c>
       <c r="AK171" t="s">
         <v>663</v>
       </c>
@@ -13608,6 +13752,12 @@
       <c r="X172" t="s">
         <v>42</v>
       </c>
+      <c r="AG172" t="s">
+        <v>1724</v>
+      </c>
+      <c r="AH172" t="s">
+        <v>42</v>
+      </c>
       <c r="AK172" t="s">
         <v>664</v>
       </c>
@@ -13622,6 +13772,12 @@
       <c r="X173" t="s">
         <v>42</v>
       </c>
+      <c r="AG173" t="s">
+        <v>1725</v>
+      </c>
+      <c r="AH173" t="s">
+        <v>42</v>
+      </c>
       <c r="AK173" t="s">
         <v>665</v>
       </c>
@@ -13636,6 +13792,12 @@
       <c r="X174" t="s">
         <v>42</v>
       </c>
+      <c r="AG174" t="s">
+        <v>1726</v>
+      </c>
+      <c r="AH174" t="s">
+        <v>42</v>
+      </c>
       <c r="AK174" t="s">
         <v>666</v>
       </c>
@@ -13650,6 +13812,12 @@
       <c r="X175" t="s">
         <v>42</v>
       </c>
+      <c r="AG175" t="s">
+        <v>1727</v>
+      </c>
+      <c r="AH175" t="s">
+        <v>42</v>
+      </c>
       <c r="AK175" t="s">
         <v>667</v>
       </c>
@@ -13664,6 +13832,12 @@
       <c r="X176" t="s">
         <v>42</v>
       </c>
+      <c r="AG176" t="s">
+        <v>1728</v>
+      </c>
+      <c r="AH176" t="s">
+        <v>42</v>
+      </c>
       <c r="AK176" t="s">
         <v>668</v>
       </c>
@@ -13678,6 +13852,12 @@
       <c r="X177" t="s">
         <v>42</v>
       </c>
+      <c r="AG177" t="s">
+        <v>1729</v>
+      </c>
+      <c r="AH177" t="s">
+        <v>42</v>
+      </c>
       <c r="AK177" t="s">
         <v>669</v>
       </c>
@@ -13692,6 +13872,12 @@
       <c r="X178" t="s">
         <v>42</v>
       </c>
+      <c r="AG178" t="s">
+        <v>1730</v>
+      </c>
+      <c r="AH178" t="s">
+        <v>42</v>
+      </c>
       <c r="AK178" t="s">
         <v>670</v>
       </c>
@@ -13706,6 +13892,12 @@
       <c r="X179" t="s">
         <v>42</v>
       </c>
+      <c r="AG179" t="s">
+        <v>1731</v>
+      </c>
+      <c r="AH179" t="s">
+        <v>42</v>
+      </c>
       <c r="AK179" t="s">
         <v>671</v>
       </c>
@@ -13720,6 +13912,12 @@
       <c r="X180" t="s">
         <v>42</v>
       </c>
+      <c r="AG180" t="s">
+        <v>1732</v>
+      </c>
+      <c r="AH180" t="s">
+        <v>42</v>
+      </c>
       <c r="AK180" t="s">
         <v>672</v>
       </c>
@@ -13734,6 +13932,12 @@
       <c r="X181" t="s">
         <v>42</v>
       </c>
+      <c r="AG181" t="s">
+        <v>1733</v>
+      </c>
+      <c r="AH181" t="s">
+        <v>42</v>
+      </c>
       <c r="AK181" t="s">
         <v>673</v>
       </c>
@@ -25055,13 +25259,13 @@
     </row>
     <row r="990" spans="23:38">
       <c r="W990" t="s">
-        <v>463</v>
+        <v>1482</v>
       </c>
       <c r="X990" t="s">
         <v>42</v>
       </c>
       <c r="AK990" t="s">
-        <v>463</v>
+        <v>1482</v>
       </c>
       <c r="AL990" t="s">
         <v>42</v>
@@ -25069,13 +25273,13 @@
     </row>
     <row r="991" spans="23:38">
       <c r="W991" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="X991" t="s">
         <v>42</v>
       </c>
       <c r="AK991" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="AL991" t="s">
         <v>42</v>
@@ -25083,13 +25287,13 @@
     </row>
     <row r="992" spans="23:38">
       <c r="W992" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="X992" t="s">
         <v>42</v>
       </c>
       <c r="AK992" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="AL992" t="s">
         <v>42</v>
@@ -25097,13 +25301,13 @@
     </row>
     <row r="993" spans="23:38">
       <c r="W993" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="X993" t="s">
         <v>42</v>
       </c>
       <c r="AK993" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="AL993" t="s">
         <v>42</v>
@@ -25111,13 +25315,13 @@
     </row>
     <row r="994" spans="23:38">
       <c r="W994" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="X994" t="s">
         <v>42</v>
       </c>
       <c r="AK994" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="AL994" t="s">
         <v>42</v>
@@ -25125,15 +25329,127 @@
     </row>
     <row r="995" spans="23:38">
       <c r="W995" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="X995" t="s">
         <v>42</v>
       </c>
       <c r="AK995" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="AL995" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="996" spans="23:38">
+      <c r="W996" t="s">
+        <v>1488</v>
+      </c>
+      <c r="X996" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK996" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AL996" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="997" spans="23:38">
+      <c r="W997" t="s">
+        <v>1489</v>
+      </c>
+      <c r="X997" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK997" t="s">
+        <v>1489</v>
+      </c>
+      <c r="AL997" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="998" spans="23:38">
+      <c r="W998" t="s">
+        <v>463</v>
+      </c>
+      <c r="X998" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK998" t="s">
+        <v>463</v>
+      </c>
+      <c r="AL998" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="999" spans="23:38">
+      <c r="W999" t="s">
+        <v>1490</v>
+      </c>
+      <c r="X999" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK999" t="s">
+        <v>1490</v>
+      </c>
+      <c r="AL999" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1000" spans="23:38">
+      <c r="W1000" t="s">
+        <v>1491</v>
+      </c>
+      <c r="X1000" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1000" t="s">
+        <v>1491</v>
+      </c>
+      <c r="AL1000" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1001" spans="23:38">
+      <c r="W1001" t="s">
+        <v>1492</v>
+      </c>
+      <c r="X1001" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1001" t="s">
+        <v>1492</v>
+      </c>
+      <c r="AL1001" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1002" spans="23:38">
+      <c r="W1002" t="s">
+        <v>1493</v>
+      </c>
+      <c r="X1002" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1002" t="s">
+        <v>1493</v>
+      </c>
+      <c r="AL1002" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1003" spans="23:38">
+      <c r="W1003" t="s">
+        <v>1494</v>
+      </c>
+      <c r="X1003" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1003" t="s">
+        <v>1494</v>
+      </c>
+      <c r="AL1003" t="s">
         <v>42</v>
       </c>
     </row>
@@ -27452,7 +27768,7 @@
   </mergeCells>
   <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8:A1000001">
-      <formula1>'Codelijsten'!$W$4:$W$995</formula1>
+      <formula1>'Codelijsten'!$W$4:$W$1003</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N8:N1000001">
       <formula1>'Codelijsten'!$Y$4:$Y$68</formula1>
@@ -27467,7 +27783,7 @@
       <formula1>'Codelijsten'!$AE$4:$AE$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD8:AD1000001">
-      <formula1>'Codelijsten'!$AG$4:$AG$161</formula1>
+      <formula1>'Codelijsten'!$AG$4:$AG$181</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE8:AE1000001">
       <formula1>-146096</formula1>
@@ -27479,7 +27795,7 @@
       <formula1>'Codelijsten'!$AI$4:$AI$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY8:AY1000001">
-      <formula1>'Codelijsten'!$AK$4:$AK$995</formula1>
+      <formula1>'Codelijsten'!$AK$4:$AK$1003</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB8:BB1000001">
       <formula1>'Codelijsten'!$AM$4:$AM$68</formula1>
@@ -27523,50 +27839,50 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>1710</v>
+        <v>1738</v>
       </c>
       <c r="B1" t="s">
-        <v>1711</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1712</v>
+        <v>1740</v>
       </c>
       <c r="B2" t="s">
-        <v>1713</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>1714</v>
+        <v>1742</v>
       </c>
       <c r="B3" t="s">
-        <v>1715</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>1716</v>
+        <v>1744</v>
       </c>
       <c r="B4" t="s">
-        <v>1717</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>1718</v>
+        <v>1746</v>
       </c>
       <c r="B5" t="s">
-        <v>1719</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>1720</v>
+        <v>1748</v>
       </c>
       <c r="B6" t="s">
-        <v>1721</v>
+        <v>1749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>